<commit_message>
Excel examples (pivot/consort tables)
</commit_message>
<xml_diff>
--- a/EXCEL_advanced/CONSORT_adv_functions.xlsx
+++ b/EXCEL_advanced/CONSORT_adv_functions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PubLibrary\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github samples\EXCEL_advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1DE959-EE38-4116-8F6F-B856E1AFF587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Randomization_Info" sheetId="2" r:id="rId1"/>
@@ -18,18 +19,29 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Randomization_Info!$A$1:$I$180</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Debby</author>
     <author>D'Angelo, Debra</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -134,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -186,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0">
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -356,7 +368,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -824,7 +836,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -836,6 +848,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,6 +862,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -865,18 +889,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,7 +927,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -970,7 +982,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1025,7 +1037,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1080,7 +1092,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1135,7 +1147,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1190,7 +1202,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,6 +1318,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1341,6 +1370,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1516,12 +1562,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N180"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6258,7 +6304,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G198">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G198">
     <sortCondition ref="A2:A198"/>
   </sortState>
   <mergeCells count="2">
@@ -6272,12 +6318,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:L43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6291,17 +6335,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="G2" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="38"/>
+      <c r="G2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="G3" s="39">
+      <c r="G3" s="43">
         <f>COUNT(Randomization_Info!A2:A180)</f>
         <v>179</v>
       </c>
-      <c r="H3" s="40"/>
+      <c r="H3" s="44"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="G4" s="3"/>
@@ -6358,43 +6402,43 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="G13" s="41">
+      <c r="G13" s="45">
         <f>COUNTIF(Randomization_Info!D2:D180, 1)</f>
         <v>89</v>
       </c>
-      <c r="H13" s="42"/>
+      <c r="H13" s="46"/>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
-      <c r="J15" s="36" t="s">
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="J15" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="40"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="48"/>
       <c r="E16" s="20">
         <f>COUNTIFS(Randomization_Info!$D$2:$D$180,1,Randomization_Info!$F$2:$F$180,"A")</f>
         <v>44</v>
       </c>
-      <c r="J16" s="43" t="s">
+      <c r="J16" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="45"/>
+      <c r="K16" s="49"/>
       <c r="L16" s="29">
         <f>COUNTIFS(Randomization_Info!$D$2:$D$180,1,Randomization_Info!$F$2:$F$180,"B")</f>
         <v>45</v>
@@ -6437,16 +6481,16 @@
       </c>
     </row>
     <row r="24" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="J24" s="36" t="s">
+      <c r="D24" s="39"/>
+      <c r="E24" s="40"/>
+      <c r="J24" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="37"/>
-      <c r="L24" s="38"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="40"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C25" s="10"/>
@@ -6485,16 +6529,16 @@
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="38"/>
-      <c r="J32" s="36" t="s">
+      <c r="D32" s="39"/>
+      <c r="E32" s="40"/>
+      <c r="J32" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="K32" s="37"/>
-      <c r="L32" s="38"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="40"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C33" s="10"/>
@@ -6533,40 +6577,40 @@
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="37"/>
-      <c r="E39" s="38"/>
-      <c r="J39" s="36" t="s">
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
+      <c r="J39" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="K39" s="37"/>
-      <c r="L39" s="38"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="40"/>
     </row>
     <row r="40" spans="3:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
-      <c r="D40" s="46" t="s">
+      <c r="D40" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="48" t="s">
+      <c r="E40" s="41" t="s">
         <v>31</v>
       </c>
       <c r="J40" s="1"/>
-      <c r="K40" s="46" t="s">
+      <c r="K40" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="L40" s="48" t="s">
+      <c r="L40" s="41" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="49"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="42"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="49"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="42"/>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C42" s="14" t="s">
@@ -6618,6 +6662,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="K40:K41"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="J24:L24"/>
@@ -6627,15 +6680,6 @@
     <mergeCell ref="J39:L39"/>
     <mergeCell ref="E40:E41"/>
     <mergeCell ref="L40:L41"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="J16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>